<commit_message>
add consistency to initial table and small error fixes
</commit_message>
<xml_diff>
--- a/efficiency-results.xlsx
+++ b/efficiency-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba5kv4\git\dissertation-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1516E771-BAA9-4E82-A5D5-DF81D341D730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB23132-C137-486F-935F-9D0FA527CA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{25DE5334-8C91-426F-A24A-6E4284BCB023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{25DE5334-8C91-426F-A24A-6E4284BCB023}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="306">
   <si>
     <t>Task</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>2025-09-21T21:18:10,generate-LSTM,ada201ce-9066-41a3-b581-bbba233a1b9b,5b0fa12a-3dd7-45bb-9766-cc326314d9f1,85003.85627300301,0.472226465998342,5.555353447515532e-06,32.5,0.0,20.0,0.7673812768170075,0.0,0.47222094394251335,1.2396022207595274,Germany,DEU,bavaria,,,Linux-6.6.87.2-microsoft-standard-WSL2-x86_64-with-glibc2.35,3.10.12,3.0.5,16,AMD Ryzen 7 7700 8-Core Processor,,,10.8922,49.8917,30.90642547607422,machine,N,1.0</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Processing took: 85590.61884953
@@ -672,18 +669,6 @@
   </si>
   <si>
     <t>2025-11-06T05:08:06,mixtral,672f349d-8ed3-4648-89f8-49d3b5e9a9f7,5b0fa12a-3dd7-45bb-9766-cc326314d9f1,124581.0286156,3.690865178487722,2.9626221741000724e-05,260.0,0.0,20.0,8.996556254219453,0.0,0.6920253929461145,9.688581647165565,Germany,DEU,bavaria,,,Windows-11-10.0.26200-SP0,3.13.2,3.0.7,8,Intel(R) Core(TM) i7-9700 CPU @ 3.00GHz,1.0,1 x NVIDIA GeForce GTX 1050 Ti,10.9678,49.8472,63.81718826293945,machine,N,1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing took: 244465.04085330002
-[codecarbon INFO @ 10:10:18] Energy consumed for RAM : 1.357931 kWh. RAM Power : 20.0 W
-[codecarbon INFO @ 10:10:18] Delta energy consumed for CPU with constant : 0.000699 kWh, power : 260.0 W
-[codecarbon INFO @ 10:10:18] Energy consumed for All CPU : 17.653527 kWh
-[codecarbon INFO @ 10:10:18] Energy consumed for all GPUs : 0.000000 kWh. Total GPU Power : 0.0 W
-[codecarbon INFO @ 10:10:18] 19.011458 kWh of electricity used since the beginning.
-</t>
-  </si>
-  <si>
-    <t>2025-10-30T10:10:18,mixtral,85b2e9b4-1c8e-499a-a6c1-25659a382ebe,5b0fa12a-3dd7-45bb-9766-cc326314d9f1,244459.7911063,7.242414814004023,2.9626200616586305e-05,260.0,0.0,20.0,17.65352670749057,0.0,1.357931000880563,19.01145770837124,Germany,DEU,bavaria,,,Windows-11-10.0.26200-SP0,3.13.2,3.0.7,8,Intel(R) Core(TM) i7-9700 CPU @ 3.00GHz,1.0,1 x NVIDIA GeForce GTX 1050 Ti,10.8334,49.9129,63.81718826293945,machine,N,1.0</t>
   </si>
   <si>
     <t>TS2/S3</t>
@@ -1488,6 +1473,17 @@
   </si>
   <si>
     <t>2025-10-24T12:25:17,mistralnemo,af24dd51-e6f5-4097-b60e-57e211070f58,5b0fa12a-3dd7-45bb-9766-cc326314d9f1,15.643080289999489,0.00042856116946968616,2.739621363087053e-05,32.5,202.35643389222045,20.0,0.00014119161574375187,0.0008969046064120079,8.688387882779758e-05,0.0011249801009835573,Germany,DEU,bavaria,,,Linux-6.6.87.2-microsoft-standard-WSL2-x86_64-with-glibc2.39,3.12.3,3.0.7,16,AMD Ryzen 7 7700 8-Core Processor,1.0,1 x NVIDIA GeForce RTX 5070 Ti,10.9678,49.8472,30.90642547607422,machine,N,1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing took: 71435.42540539999
+[codecarbon INFO @ 17:30:40] Energy consumed for RAM : 0.396795 kWh. RAM Power : 20.0 W 
+[codecarbon INFO @ 17:30:40] Delta energy consumed for CPU with constant : 0.001015 kWh, power : 260.0 W 
+[codecarbon INFO @ 17:30:40] Energy consumed for All CPU : 5.158466 kWh 
+[codecarbon INFO @ 17:30:40] Energy consumed for all GPUs : 0.000000 kWh. Total GPU Power : 0.0 W 
+[codecarbon INFO @ 17:30:40] 5.555261 kWh of electricity used since the beginning. </t>
+  </si>
+  <si>
+    <t>2026-01-07T17:30:40,mixtral,bab8f5f5-12a2-46ae-823c-ef67a62b9858,5b0fa12a-3dd7-45bb-9766-cc326314d9f1,71432.7083403,2.1162766037610594,2.962615660152879e-05,260.0,0.0,20.0,5.158466053000027,0.0,0.3967947522527783,5.555260805252813,Germany,DEU,bavaria,,,Windows-11-10.0.26200-SP0,3.13.2,3.0.7,8,Intel(R) Core(TM) i7-9700 CPU @ 3.00GHz,1,1 x NVIDIA GeForce GTX 1050 Ti,10.9545,49.9282,63.81718826293945,machine,N,1.0</t>
   </si>
 </sst>
 </file>
@@ -1898,31 +1894,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6EA777-CF04-4C7B-A34F-611A2B3B8ABF}">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116:S118"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1981,7 +1979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2042,7 +2040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2164,7 +2162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2225,7 +2223,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2286,7 +2284,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2347,7 +2345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2408,7 +2406,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2467,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2528,7 +2526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2589,7 +2587,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2649,7 +2647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2709,7 +2707,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2769,7 +2767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2891,7 +2889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +2950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2969,7 +2967,7 @@
         <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G20" t="str">
         <f>"/code/"&amp;"NLG-"&amp;E20&amp;"/lstm_gpu"</f>
@@ -2980,7 +2978,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
-        <v>/output/NLG/S3/LSTM/yes</v>
+        <v>/output/NLG/S3/LSTM/GPU</v>
       </c>
       <c r="J20">
         <v>85590.618849530001</v>
@@ -3007,13 +3005,13 @@
         <v>20</v>
       </c>
       <c r="R20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" t="s">
         <v>62</v>
       </c>
-      <c r="S20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3068,13 +3066,13 @@
         <v>11.589908123016301</v>
       </c>
       <c r="R21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S21" t="s">
         <v>64</v>
       </c>
-      <c r="S21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3091,7 +3089,7 @@
         <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G22" t="str">
         <f>"/code/"&amp;"NLG-"&amp;E22&amp;"/gpt"</f>
@@ -3102,7 +3100,7 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
-        <v>/output/NLG/S3/GPT-2/yes</v>
+        <v>/output/NLG/S3/GPT-2/GPU</v>
       </c>
       <c r="J22">
         <v>3627.2578113589898</v>
@@ -3129,13 +3127,13 @@
         <v>20</v>
       </c>
       <c r="R22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S22" t="s">
         <v>66</v>
       </c>
-      <c r="S22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3190,13 +3188,13 @@
         <v>11.5899095535278</v>
       </c>
       <c r="R23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S23" t="s">
         <v>68</v>
       </c>
-      <c r="S23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3213,7 +3211,7 @@
         <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G24" t="str">
         <f>"/code/"&amp;"NLG-"&amp;E24&amp;"/gptfine"</f>
@@ -3224,7 +3222,7 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
-        <v>/output/NLG/S3/GPT-2-Finetuned/yes</v>
+        <v>/output/NLG/S3/GPT-2-Finetuned/GPU</v>
       </c>
       <c r="J24">
         <v>5349.3007802120001</v>
@@ -3251,21 +3249,21 @@
         <v>20</v>
       </c>
       <c r="R24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S24" t="s">
         <v>70</v>
       </c>
-      <c r="S24" t="s">
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>73</v>
-      </c>
-      <c r="C27" t="s">
-        <v>74</v>
       </c>
       <c r="D27" s="3">
         <v>45925</v>
@@ -3281,7 +3279,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -3312,21 +3310,21 @@
         <v>10</v>
       </c>
       <c r="R27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="S27" t="s">
         <v>76</v>
       </c>
-      <c r="S27" t="s">
+    </row>
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
       </c>
       <c r="D28" s="3">
         <v>45925</v>
@@ -3342,7 +3340,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -3373,21 +3371,21 @@
         <v>10</v>
       </c>
       <c r="R28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="S28" t="s">
         <v>79</v>
       </c>
-      <c r="S28" t="s">
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
       </c>
       <c r="D29" s="3">
         <v>45924</v>
@@ -3403,7 +3401,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -3434,21 +3432,21 @@
         <v>10</v>
       </c>
       <c r="R29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S29" t="s">
         <v>82</v>
       </c>
-      <c r="S29" t="s">
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
       </c>
       <c r="D30" s="3">
         <v>45924</v>
@@ -3464,7 +3462,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -3495,21 +3493,21 @@
         <v>10</v>
       </c>
       <c r="R30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="S30" t="s">
         <v>85</v>
       </c>
-      <c r="S30" t="s">
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>87</v>
       </c>
       <c r="D31" s="3">
         <v>45924</v>
@@ -3525,7 +3523,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
@@ -3556,21 +3554,21 @@
         <v>10</v>
       </c>
       <c r="R31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="S31" t="s">
         <v>88</v>
       </c>
-      <c r="S31" t="s">
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
       </c>
       <c r="D32" s="3">
         <v>45924</v>
@@ -3586,7 +3584,7 @@
         <v>/code/TS1-S1</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -3617,21 +3615,21 @@
         <v>10</v>
       </c>
       <c r="R32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S32" t="s">
         <v>91</v>
       </c>
-      <c r="S32" t="s">
+    </row>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
-      </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34" s="3">
         <v>45968</v>
@@ -3647,7 +3645,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
@@ -3678,21 +3676,21 @@
         <v>20</v>
       </c>
       <c r="R34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="S34" t="s">
         <v>94</v>
       </c>
-      <c r="S34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3">
         <v>45968</v>
@@ -3708,7 +3706,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
@@ -3739,21 +3737,21 @@
         <v>20</v>
       </c>
       <c r="R35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="S35" t="s">
         <v>96</v>
       </c>
-      <c r="S35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="3">
         <v>45967</v>
@@ -3769,7 +3767,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
@@ -3800,21 +3798,21 @@
         <v>20</v>
       </c>
       <c r="R36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="S36" t="s">
         <v>98</v>
       </c>
-      <c r="S36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
@@ -3865,15 +3863,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3">
         <v>45968</v>
@@ -3889,7 +3887,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
@@ -3920,21 +3918,21 @@
         <v>20</v>
       </c>
       <c r="R38" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="S38" t="s">
         <v>100</v>
       </c>
-      <c r="S38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
         <v>25</v>
@@ -3985,15 +3983,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="3">
         <v>45968</v>
@@ -4009,7 +4007,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
@@ -4040,21 +4038,21 @@
         <v>20</v>
       </c>
       <c r="R40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="S40" t="s">
         <v>102</v>
       </c>
-      <c r="S40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
@@ -4105,15 +4103,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="3">
         <v>45968</v>
@@ -4129,7 +4127,7 @@
         <v>/code/TS1-S2</v>
       </c>
       <c r="H42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
@@ -4160,21 +4158,21 @@
         <v>20</v>
       </c>
       <c r="R42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="S42" t="s">
         <v>104</v>
       </c>
-      <c r="S42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
         <v>25</v>
@@ -4226,15 +4224,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="3">
         <v>45959</v>
@@ -4250,7 +4248,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
@@ -4281,21 +4279,21 @@
         <v>20</v>
       </c>
       <c r="R45" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="S45" t="s">
         <v>107</v>
       </c>
-      <c r="S45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="3">
         <v>45959</v>
@@ -4311,7 +4309,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="0"/>
@@ -4342,21 +4340,21 @@
         <v>20</v>
       </c>
       <c r="R46" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="S46" t="s">
         <v>109</v>
       </c>
-      <c r="S46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D47" s="3">
         <v>45968</v>
@@ -4372,7 +4370,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
@@ -4403,21 +4401,21 @@
         <v>20</v>
       </c>
       <c r="R47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="S47" t="s">
         <v>111</v>
       </c>
-      <c r="S47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" s="3">
         <v>45959</v>
@@ -4433,7 +4431,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
@@ -4464,21 +4462,21 @@
         <v>20</v>
       </c>
       <c r="R48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="S48" t="s">
         <v>113</v>
       </c>
-      <c r="S48" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" s="3">
         <v>45968</v>
@@ -4494,7 +4492,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
@@ -4525,21 +4523,21 @@
         <v>20</v>
       </c>
       <c r="R49" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="S49" t="s">
         <v>115</v>
       </c>
-      <c r="S49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D50" s="3">
         <v>45967</v>
@@ -4555,7 +4553,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
@@ -4586,21 +4584,21 @@
         <v>20</v>
       </c>
       <c r="R50" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="S50" t="s">
         <v>117</v>
       </c>
-      <c r="S50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="3">
         <v>45968</v>
@@ -4616,7 +4614,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
@@ -4647,21 +4645,21 @@
         <v>20</v>
       </c>
       <c r="R51" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="S51" t="s">
         <v>119</v>
       </c>
-      <c r="S51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D52" s="3">
         <v>45959</v>
@@ -4677,7 +4675,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="0"/>
@@ -4708,21 +4706,21 @@
         <v>20</v>
       </c>
       <c r="R52" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="S52" t="s">
         <v>121</v>
       </c>
-      <c r="S52" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="3">
         <v>45968</v>
@@ -4738,7 +4736,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="0"/>
@@ -4769,21 +4767,21 @@
         <v>20</v>
       </c>
       <c r="R53" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="S53" t="s">
         <v>123</v>
       </c>
-      <c r="S53" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D54" s="3">
         <v>45967</v>
@@ -4799,7 +4797,7 @@
         <v>/code/TS1-S3</v>
       </c>
       <c r="H54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="0"/>
@@ -4830,21 +4828,21 @@
         <v>20</v>
       </c>
       <c r="R54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="S54" t="s">
         <v>125</v>
       </c>
-      <c r="S54" t="s">
+    </row>
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
         <v>127</v>
       </c>
-      <c r="B57" t="s">
-        <v>128</v>
-      </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D57" s="3">
         <v>45943</v>
@@ -4860,7 +4858,7 @@
         <v>/code/TS2-S1/lex</v>
       </c>
       <c r="H57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="0"/>
@@ -4891,21 +4889,21 @@
         <v>10</v>
       </c>
       <c r="R57" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="S57" t="s">
         <v>130</v>
       </c>
-      <c r="S57" t="s">
+    </row>
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" t="s">
-        <v>128</v>
-      </c>
-      <c r="C58" t="s">
-        <v>132</v>
       </c>
       <c r="D58" s="3">
         <v>45943</v>
@@ -4921,7 +4919,7 @@
         <v>/code/TS2-S1/bert2bert</v>
       </c>
       <c r="H58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="0"/>
@@ -4952,21 +4950,21 @@
         <v>10</v>
       </c>
       <c r="R58" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S58" t="s">
         <v>133</v>
       </c>
-      <c r="S58" t="s">
+    </row>
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" t="s">
-        <v>135</v>
       </c>
       <c r="D59" s="3">
         <v>45975</v>
@@ -4982,7 +4980,7 @@
         <v>/code/TS2-S1/mlong</v>
       </c>
       <c r="H59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="0"/>
@@ -5013,21 +5011,21 @@
         <v>10</v>
       </c>
       <c r="R59" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="S59" t="s">
         <v>136</v>
       </c>
-      <c r="S59" t="s">
+    </row>
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" t="s">
-        <v>138</v>
       </c>
       <c r="D60" s="3">
         <v>45950</v>
@@ -5043,7 +5041,7 @@
         <v>/code/TS2-S1/mixtral</v>
       </c>
       <c r="H60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="0"/>
@@ -5074,21 +5072,21 @@
         <v>20</v>
       </c>
       <c r="R60" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S60" t="s">
         <v>139</v>
       </c>
-      <c r="S60" t="s">
+    </row>
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" t="s">
-        <v>141</v>
-      </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" s="3">
         <v>45964</v>
@@ -5104,7 +5102,7 @@
         <v>/code/TS2-S2/lex</v>
       </c>
       <c r="H62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="0"/>
@@ -5135,21 +5133,21 @@
         <v>20</v>
       </c>
       <c r="R62" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="S62" t="s">
         <v>142</v>
       </c>
-      <c r="S62" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D63" s="3">
         <v>45944</v>
@@ -5165,7 +5163,7 @@
         <v>/code/TS2-S2/bert2bert</v>
       </c>
       <c r="H63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="0"/>
@@ -5196,21 +5194,21 @@
         <v>20</v>
       </c>
       <c r="R63" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="S63" t="s">
         <v>144</v>
       </c>
-      <c r="S63" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
         <v>25</v>
@@ -5261,15 +5259,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D65" s="3">
         <v>45975</v>
@@ -5285,7 +5283,7 @@
         <v>/code/TS2-S2/mlong</v>
       </c>
       <c r="H65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="0"/>
@@ -5316,21 +5314,21 @@
         <v>20</v>
       </c>
       <c r="R65" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S65" t="s">
         <v>146</v>
       </c>
-      <c r="S65" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
         <v>25</v>
@@ -5381,15 +5379,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" s="3">
         <v>45967</v>
@@ -5405,7 +5403,7 @@
         <v>/code/TS2-S2/mixtral</v>
       </c>
       <c r="H67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I130" si="3">"/output/"&amp;B67&amp;"/"&amp;C67&amp;"/"&amp;F67</f>
@@ -5430,24 +5428,24 @@
         <v>20</v>
       </c>
       <c r="R67" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="S67" t="s">
         <v>148</v>
       </c>
-      <c r="S67" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D68" s="3">
-        <v>45960</v>
+        <v>46028</v>
       </c>
       <c r="E68" t="s">
         <v>41</v>
@@ -5460,46 +5458,52 @@
         <v>/code/TS2-S2/mixtral</v>
       </c>
       <c r="H68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I68" t="str">
         <f t="shared" si="3"/>
         <v>/output/TS2/S2/Mistral/GPU</v>
       </c>
       <c r="J68">
-        <v>244465.04085329999</v>
+        <v>71435.425405399903</v>
       </c>
       <c r="K68">
-        <v>19.011458000000001</v>
+        <v>5.5552609999999998</v>
       </c>
       <c r="L68">
-        <v>17.653527</v>
+        <v>5.1584659999999998</v>
       </c>
       <c r="M68">
         <v>260</v>
       </c>
+      <c r="N68" t="s">
+        <v>25</v>
+      </c>
+      <c r="O68" t="s">
+        <v>25</v>
+      </c>
       <c r="P68">
-        <v>1.357931</v>
+        <v>0.39679500000000001</v>
       </c>
       <c r="Q68">
         <v>20</v>
       </c>
       <c r="R68" s="4" t="s">
-        <v>150</v>
+        <v>304</v>
       </c>
       <c r="S68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D70" s="3">
         <v>45943</v>
@@ -5515,7 +5519,7 @@
         <v>/code/TS2-S3/lex</v>
       </c>
       <c r="H70" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="3"/>
@@ -5546,21 +5550,21 @@
         <v>20</v>
       </c>
       <c r="R70" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D71" s="3">
         <v>45943</v>
@@ -5576,7 +5580,7 @@
         <v>/code/TS2-S3/bert2bert</v>
       </c>
       <c r="H71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="3"/>
@@ -5607,21 +5611,21 @@
         <v>20</v>
       </c>
       <c r="R71" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="S71" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D72" s="3">
         <v>45942</v>
@@ -5637,7 +5641,7 @@
         <v>/code/TS2-S3/bert2bert</v>
       </c>
       <c r="H72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="3"/>
@@ -5668,21 +5672,21 @@
         <v>20</v>
       </c>
       <c r="R72" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="S72" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D73" s="3">
         <v>45975</v>
@@ -5698,7 +5702,7 @@
         <v>/code/TS2-S3/mlong</v>
       </c>
       <c r="H73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I73" t="str">
         <f t="shared" si="3"/>
@@ -5729,21 +5733,21 @@
         <v>20</v>
       </c>
       <c r="R73" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S73" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D74" s="3">
         <v>45975</v>
@@ -5759,7 +5763,7 @@
         <v>/code/TS2-S3/mlong</v>
       </c>
       <c r="H74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="3"/>
@@ -5790,21 +5794,21 @@
         <v>20</v>
       </c>
       <c r="R74" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="S74" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D75" s="3">
         <v>45947</v>
@@ -5820,7 +5824,7 @@
         <v>/code/TS2-S3/mixtral</v>
       </c>
       <c r="H75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I75" t="str">
         <f t="shared" si="3"/>
@@ -5851,21 +5855,21 @@
         <v>20</v>
       </c>
       <c r="R75" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="S75" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D76" s="3">
         <v>45975</v>
@@ -5881,7 +5885,7 @@
         <v>/code/TS2-S3/mixtral</v>
       </c>
       <c r="H76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I76" t="str">
         <f t="shared" si="3"/>
@@ -5912,21 +5916,21 @@
         <v>20</v>
       </c>
       <c r="R76" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" t="s">
         <v>165</v>
       </c>
-      <c r="S76" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>167</v>
-      </c>
-      <c r="B79" t="s">
-        <v>168</v>
-      </c>
       <c r="C79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D79" s="3">
         <v>45947</v>
@@ -5942,7 +5946,7 @@
         <v>/code/TS3-S1/lexrank</v>
       </c>
       <c r="H79" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="3"/>
@@ -5973,21 +5977,21 @@
         <v>10</v>
       </c>
       <c r="R79" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="S79" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B80" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D80" s="3">
         <v>45947</v>
@@ -6003,7 +6007,7 @@
         <v>/code/TS3-S1/lexrank</v>
       </c>
       <c r="H80" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="3"/>
@@ -6034,21 +6038,21 @@
         <v>10</v>
       </c>
       <c r="R80" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="S80" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D81" s="3">
         <v>45947</v>
@@ -6064,7 +6068,7 @@
         <v>/code/TS3-S1/lexrank</v>
       </c>
       <c r="H81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I81" t="str">
         <f t="shared" si="3"/>
@@ -6095,21 +6099,21 @@
         <v>10</v>
       </c>
       <c r="R81" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="S81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D82" s="3">
         <v>45947</v>
@@ -6125,7 +6129,7 @@
         <v>/code/TS3-S1/lexrank</v>
       </c>
       <c r="H82" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I82" t="str">
         <f t="shared" si="3"/>
@@ -6156,21 +6160,21 @@
         <v>10</v>
       </c>
       <c r="R82" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="S82" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D83" s="3">
         <v>45947</v>
@@ -6186,7 +6190,7 @@
         <v>/code/TS3-S1/lexrank</v>
       </c>
       <c r="H83" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" si="3"/>
@@ -6217,21 +6221,21 @@
         <v>10</v>
       </c>
       <c r="R83" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S83" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B84" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D84" s="3">
         <v>45952</v>
@@ -6247,7 +6251,7 @@
         <v>/code/TS3-S1/mlongt5</v>
       </c>
       <c r="H84" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I84" t="str">
         <f t="shared" si="3"/>
@@ -6278,21 +6282,21 @@
         <v>10</v>
       </c>
       <c r="R84" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S84" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D85" s="3">
         <v>45952</v>
@@ -6308,7 +6312,7 @@
         <v>/code/TS3-S1/mlongt5</v>
       </c>
       <c r="H85" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" si="3"/>
@@ -6339,21 +6343,21 @@
         <v>10</v>
       </c>
       <c r="R85" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="S85" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D86" s="3">
         <v>45952</v>
@@ -6369,7 +6373,7 @@
         <v>/code/TS3-S1/mlongt5</v>
       </c>
       <c r="H86" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I86" t="str">
         <f t="shared" si="3"/>
@@ -6400,21 +6404,21 @@
         <v>10</v>
       </c>
       <c r="R86" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="S86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D87" s="3">
         <v>45952</v>
@@ -6430,7 +6434,7 @@
         <v>/code/TS3-S1/mlongt5</v>
       </c>
       <c r="H87" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I87" t="str">
         <f t="shared" si="3"/>
@@ -6461,21 +6465,21 @@
         <v>10</v>
       </c>
       <c r="R87" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S87" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D88" s="3">
         <v>45952</v>
@@ -6491,7 +6495,7 @@
         <v>/code/TS3-S1/mlongt5</v>
       </c>
       <c r="H88" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I88" t="str">
         <f t="shared" si="3"/>
@@ -6522,21 +6526,21 @@
         <v>10</v>
       </c>
       <c r="R88" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="S88" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C89" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D89" s="3">
         <v>45952</v>
@@ -6552,7 +6556,7 @@
         <v>/code/TS3-S1/mistralnemo</v>
       </c>
       <c r="H89" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I89" t="str">
         <f t="shared" si="3"/>
@@ -6583,21 +6587,21 @@
         <v>10</v>
       </c>
       <c r="R89" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="S89" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B90" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C90" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D90" s="3">
         <v>45952</v>
@@ -6613,7 +6617,7 @@
         <v>/code/TS3-S1/mistralnemo</v>
       </c>
       <c r="H90" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I90" t="str">
         <f t="shared" si="3"/>
@@ -6644,21 +6648,21 @@
         <v>10</v>
       </c>
       <c r="R90" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S90" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C91" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D91" s="3">
         <v>45952</v>
@@ -6674,7 +6678,7 @@
         <v>/code/TS3-S1/mistralnemo</v>
       </c>
       <c r="H91" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I91" t="str">
         <f t="shared" si="3"/>
@@ -6705,21 +6709,21 @@
         <v>10</v>
       </c>
       <c r="R91" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="S91" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B92" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C92" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D92" s="3">
         <v>45956</v>
@@ -6735,7 +6739,7 @@
         <v>/code/TS3-S1/mistralnemo</v>
       </c>
       <c r="H92" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I92" t="str">
         <f t="shared" si="3"/>
@@ -6766,21 +6770,21 @@
         <v>10</v>
       </c>
       <c r="R92" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="S92" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B93" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D93" s="3">
         <v>45956</v>
@@ -6796,7 +6800,7 @@
         <v>/code/TS3-S1/mistralnemo</v>
       </c>
       <c r="H93" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I93" t="str">
         <f t="shared" si="3"/>
@@ -6827,21 +6831,21 @@
         <v>10</v>
       </c>
       <c r="R93" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="S93" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B96" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D96" s="3">
         <v>45974</v>
@@ -6857,7 +6861,7 @@
         <v>/code/TS3-S2/lexrank</v>
       </c>
       <c r="H96" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I96" t="str">
         <f t="shared" si="3"/>
@@ -6888,21 +6892,21 @@
         <v>20</v>
       </c>
       <c r="R96" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="S96" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D97" s="3">
         <v>45974</v>
@@ -6918,7 +6922,7 @@
         <v>/code/TS3-S2/lexrank</v>
       </c>
       <c r="H97" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I97" t="str">
         <f t="shared" si="3"/>
@@ -6949,21 +6953,21 @@
         <v>20</v>
       </c>
       <c r="R97" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="S97" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D98" s="3">
         <v>45974</v>
@@ -6979,7 +6983,7 @@
         <v>/code/TS3-S2/lexrank</v>
       </c>
       <c r="H98" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I98" t="str">
         <f t="shared" si="3"/>
@@ -7010,21 +7014,21 @@
         <v>20</v>
       </c>
       <c r="R98" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="S98" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D99" s="3">
         <v>45974</v>
@@ -7040,7 +7044,7 @@
         <v>/code/TS3-S2/lexrank</v>
       </c>
       <c r="H99" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I99" t="str">
         <f t="shared" si="3"/>
@@ -7071,21 +7075,21 @@
         <v>20</v>
       </c>
       <c r="R99" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="S99" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D100" s="3">
         <v>45974</v>
@@ -7101,7 +7105,7 @@
         <v>/code/TS3-S2/lexrank</v>
       </c>
       <c r="H100" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I100" t="str">
         <f t="shared" si="3"/>
@@ -7132,21 +7136,21 @@
         <v>20</v>
       </c>
       <c r="R100" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="S100" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D101" s="3">
         <v>45975</v>
@@ -7162,7 +7166,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H101" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I101" t="str">
         <f t="shared" si="3"/>
@@ -7193,21 +7197,21 @@
         <v>20</v>
       </c>
       <c r="R101" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="S101" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C102" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D102" s="3">
         <v>45975</v>
@@ -7223,7 +7227,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H102" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I102" t="str">
         <f t="shared" si="3"/>
@@ -7254,21 +7258,21 @@
         <v>20</v>
       </c>
       <c r="R102" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="S102" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="103" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D103" s="3">
         <v>45974</v>
@@ -7284,7 +7288,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H103" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I103" t="str">
         <f t="shared" si="3"/>
@@ -7315,21 +7319,21 @@
         <v>20</v>
       </c>
       <c r="R103" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S103" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B104" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C104" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D104" s="3">
         <v>45974</v>
@@ -7345,7 +7349,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H104" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I104" t="str">
         <f t="shared" si="3"/>
@@ -7376,21 +7380,21 @@
         <v>20</v>
       </c>
       <c r="R104" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="S104" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="105" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B105" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D105" s="3">
         <v>45974</v>
@@ -7406,7 +7410,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H105" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I105" t="str">
         <f t="shared" si="3"/>
@@ -7437,21 +7441,21 @@
         <v>20</v>
       </c>
       <c r="R105" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="S105" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B106" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D106" s="3">
         <v>45974</v>
@@ -7467,7 +7471,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H106" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I106" t="str">
         <f t="shared" si="3"/>
@@ -7498,21 +7502,21 @@
         <v>20</v>
       </c>
       <c r="R106" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S106" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C107" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D107" s="3">
         <v>45974</v>
@@ -7528,7 +7532,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H107" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I107" t="str">
         <f t="shared" si="3"/>
@@ -7559,21 +7563,21 @@
         <v>20</v>
       </c>
       <c r="R107" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="S107" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="108" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B108" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C108" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D108" s="3">
         <v>45974</v>
@@ -7589,7 +7593,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H108" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I108" t="str">
         <f t="shared" si="3"/>
@@ -7620,21 +7624,21 @@
         <v>20</v>
       </c>
       <c r="R108" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="S108" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B109" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D109" s="3">
         <v>45974</v>
@@ -7650,7 +7654,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H109" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I109" t="str">
         <f t="shared" si="3"/>
@@ -7681,21 +7685,21 @@
         <v>20</v>
       </c>
       <c r="R109" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="S109" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B110" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D110" s="3">
         <v>45974</v>
@@ -7711,7 +7715,7 @@
         <v>/code/TS3-S2/mlongt5</v>
       </c>
       <c r="H110" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I110" t="str">
         <f t="shared" si="3"/>
@@ -7742,21 +7746,21 @@
         <v>20</v>
       </c>
       <c r="R110" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="S110" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="111" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B111" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C111" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D111" s="3">
         <v>45974</v>
@@ -7772,7 +7776,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H111" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I111" t="str">
         <f t="shared" si="3"/>
@@ -7803,21 +7807,21 @@
         <v>20</v>
       </c>
       <c r="R111" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S111" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="112" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B112" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C112" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D112" s="3">
         <v>45973</v>
@@ -7833,7 +7837,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H112" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I112" t="str">
         <f t="shared" si="3"/>
@@ -7864,21 +7868,21 @@
         <v>20</v>
       </c>
       <c r="R112" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S112" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B113" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C113" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D113" s="3">
         <v>45974</v>
@@ -7894,7 +7898,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H113" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I113" t="str">
         <f t="shared" si="3"/>
@@ -7925,21 +7929,21 @@
         <v>20</v>
       </c>
       <c r="R113" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="S113" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="114" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B114" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C114" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D114" s="3">
         <v>45974</v>
@@ -7955,7 +7959,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H114" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I114" t="str">
         <f t="shared" si="3"/>
@@ -7986,21 +7990,21 @@
         <v>20</v>
       </c>
       <c r="R114" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="S114" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="115" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B115" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D115" s="3">
         <v>45974</v>
@@ -8016,7 +8020,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H115" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I115" t="str">
         <f t="shared" si="3"/>
@@ -8047,21 +8051,21 @@
         <v>20</v>
       </c>
       <c r="R115" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="S115" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="116" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B116" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C116" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D116" s="3">
         <v>45973</v>
@@ -8077,7 +8081,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H116" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I116" t="str">
         <f t="shared" si="3"/>
@@ -8108,21 +8112,21 @@
         <v>20</v>
       </c>
       <c r="R116" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="S116" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B117" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C117" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D117" s="3">
         <v>45974</v>
@@ -8138,7 +8142,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H117" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I117" t="str">
         <f t="shared" si="3"/>
@@ -8169,21 +8173,21 @@
         <v>20</v>
       </c>
       <c r="R117" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="S117" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="118" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B118" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C118" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D118" s="3">
         <v>45973</v>
@@ -8199,7 +8203,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H118" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I118" t="str">
         <f t="shared" si="3"/>
@@ -8230,21 +8234,21 @@
         <v>20</v>
       </c>
       <c r="R118" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="S118" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B119" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C119" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D119" s="3">
         <v>45974</v>
@@ -8260,7 +8264,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H119" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I119" t="str">
         <f t="shared" si="3"/>
@@ -8291,21 +8295,21 @@
         <v>20</v>
       </c>
       <c r="R119" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="S119" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="120" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B120" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C120" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D120" s="3">
         <v>45973</v>
@@ -8321,7 +8325,7 @@
         <v>/code/TS3-S2/mistralnemo</v>
       </c>
       <c r="H120" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I120" t="str">
         <f t="shared" si="3"/>
@@ -8352,21 +8356,21 @@
         <v>20</v>
       </c>
       <c r="R120" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="S120" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D122" s="3">
         <v>45954</v>
@@ -8382,7 +8386,7 @@
         <v>/code/TS3-S3/lexrank</v>
       </c>
       <c r="H122" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I122" t="str">
         <f t="shared" si="3"/>
@@ -8413,21 +8417,21 @@
         <v>20</v>
       </c>
       <c r="R122" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="S122" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B123" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C123" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D123" s="3">
         <v>45954</v>
@@ -8443,7 +8447,7 @@
         <v>/code/TS3-S3/lexrank</v>
       </c>
       <c r="H123" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I123" t="str">
         <f t="shared" si="3"/>
@@ -8474,21 +8478,21 @@
         <v>20</v>
       </c>
       <c r="R123" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="S123" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="124" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C124" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D124" s="3">
         <v>45954</v>
@@ -8504,7 +8508,7 @@
         <v>/code/TS3-S3/lexrank</v>
       </c>
       <c r="H124" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I124" t="str">
         <f t="shared" si="3"/>
@@ -8535,21 +8539,21 @@
         <v>20</v>
       </c>
       <c r="R124" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="S124" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="125" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B125" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C125" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D125" s="3">
         <v>45954</v>
@@ -8565,7 +8569,7 @@
         <v>/code/TS3-S3/lexrank</v>
       </c>
       <c r="H125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I125" t="str">
         <f t="shared" si="3"/>
@@ -8596,21 +8600,21 @@
         <v>20</v>
       </c>
       <c r="R125" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="S125" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B126" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C126" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D126" s="3">
         <v>45954</v>
@@ -8626,7 +8630,7 @@
         <v>/code/TS3-S3/lexrank</v>
       </c>
       <c r="H126" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I126" t="str">
         <f t="shared" si="3"/>
@@ -8657,21 +8661,21 @@
         <v>20</v>
       </c>
       <c r="R126" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="S126" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="127" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D127" s="3">
         <v>45954</v>
@@ -8687,7 +8691,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H127" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I127" t="str">
         <f t="shared" si="3"/>
@@ -8718,21 +8722,21 @@
         <v>20</v>
       </c>
       <c r="R127" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="S127" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="128" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C128" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D128" s="3">
         <v>45954</v>
@@ -8748,7 +8752,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H128" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I128" t="str">
         <f t="shared" si="3"/>
@@ -8779,21 +8783,21 @@
         <v>20</v>
       </c>
       <c r="R128" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="S128" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="129" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D129" s="3">
         <v>45954</v>
@@ -8809,7 +8813,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I129" t="str">
         <f t="shared" si="3"/>
@@ -8840,21 +8844,21 @@
         <v>20</v>
       </c>
       <c r="R129" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="S129" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D130" s="3">
         <v>45954</v>
@@ -8870,7 +8874,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H130" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I130" t="str">
         <f t="shared" si="3"/>
@@ -8901,21 +8905,21 @@
         <v>20</v>
       </c>
       <c r="R130" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="S130" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="131" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D131" s="3">
         <v>45954</v>
@@ -8931,7 +8935,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H131" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I131" t="str">
         <f t="shared" ref="I131:I146" si="10">"/output/"&amp;B131&amp;"/"&amp;C131&amp;"/"&amp;F131</f>
@@ -8962,21 +8966,21 @@
         <v>20</v>
       </c>
       <c r="R131" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="S131" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="132" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B132" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D132" s="3">
         <v>45954</v>
@@ -8992,7 +8996,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H132" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I132" t="str">
         <f t="shared" si="10"/>
@@ -9023,21 +9027,21 @@
         <v>20</v>
       </c>
       <c r="R132" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="S132" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B133" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C133" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D133" s="3">
         <v>45954</v>
@@ -9053,7 +9057,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H133" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I133" t="str">
         <f t="shared" si="10"/>
@@ -9084,21 +9088,21 @@
         <v>20</v>
       </c>
       <c r="R133" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="S133" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="134" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C134" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D134" s="3">
         <v>45954</v>
@@ -9114,7 +9118,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H134" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I134" t="str">
         <f t="shared" si="10"/>
@@ -9145,21 +9149,21 @@
         <v>20</v>
       </c>
       <c r="R134" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="S134" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="135" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B135" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D135" s="3">
         <v>45954</v>
@@ -9175,7 +9179,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H135" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I135" t="str">
         <f t="shared" si="10"/>
@@ -9206,21 +9210,21 @@
         <v>20</v>
       </c>
       <c r="R135" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="S135" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="136" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B136" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D136" s="3">
         <v>45954</v>
@@ -9236,7 +9240,7 @@
         <v>/code/TS3-S3/mlongt5</v>
       </c>
       <c r="H136" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I136" t="str">
         <f t="shared" si="10"/>
@@ -9267,21 +9271,21 @@
         <v>20</v>
       </c>
       <c r="R136" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="S136" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B137" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C137" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D137" s="3">
         <v>45954</v>
@@ -9297,7 +9301,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H137" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I137" t="str">
         <f t="shared" si="10"/>
@@ -9328,21 +9332,21 @@
         <v>20</v>
       </c>
       <c r="R137" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="S137" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="138" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B138" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C138" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D138" s="3">
         <v>45954</v>
@@ -9358,7 +9362,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H138" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I138" t="str">
         <f t="shared" si="10"/>
@@ -9389,21 +9393,21 @@
         <v>20</v>
       </c>
       <c r="R138" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="S138" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="139" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B139" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C139" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D139" s="3">
         <v>45954</v>
@@ -9419,7 +9423,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H139" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I139" t="str">
         <f t="shared" si="10"/>
@@ -9450,21 +9454,21 @@
         <v>20</v>
       </c>
       <c r="R139" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="S139" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="140" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B140" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C140" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D140" s="3">
         <v>45954</v>
@@ -9480,7 +9484,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H140" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I140" t="str">
         <f t="shared" si="10"/>
@@ -9511,21 +9515,21 @@
         <v>20</v>
       </c>
       <c r="R140" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="S140" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B141" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C141" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D141" s="3">
         <v>45954</v>
@@ -9541,7 +9545,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H141" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I141" t="str">
         <f t="shared" si="10"/>
@@ -9572,21 +9576,21 @@
         <v>20</v>
       </c>
       <c r="R141" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="S141" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="142" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B142" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C142" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D142" s="3">
         <v>45954</v>
@@ -9602,7 +9606,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H142" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I142" t="str">
         <f t="shared" si="10"/>
@@ -9633,21 +9637,21 @@
         <v>20</v>
       </c>
       <c r="R142" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="S142" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="143" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B143" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C143" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D143" s="3">
         <v>45954</v>
@@ -9663,7 +9667,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H143" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I143" t="str">
         <f t="shared" si="10"/>
@@ -9694,21 +9698,21 @@
         <v>20</v>
       </c>
       <c r="R143" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="S143" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="144" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B144" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C144" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D144" s="3">
         <v>45954</v>
@@ -9724,7 +9728,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H144" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I144" t="str">
         <f t="shared" si="10"/>
@@ -9755,21 +9759,21 @@
         <v>20</v>
       </c>
       <c r="R144" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="S144" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="145" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B145" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C145" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D145" s="3">
         <v>45954</v>
@@ -9785,7 +9789,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H145" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I145" t="str">
         <f t="shared" si="10"/>
@@ -9816,21 +9820,21 @@
         <v>20</v>
       </c>
       <c r="R145" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="S145" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="146" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B146" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C146" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D146" s="3">
         <v>45954</v>
@@ -9846,7 +9850,7 @@
         <v>/code/TS3-S3/mistralnemo</v>
       </c>
       <c r="H146" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I146" t="str">
         <f t="shared" si="10"/>
@@ -9877,10 +9881,10 @@
         <v>20</v>
       </c>
       <c r="R146" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="S146" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aligned files to each other
</commit_message>
<xml_diff>
--- a/efficiency-results.xlsx
+++ b/efficiency-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba5kv4\git\dissertation-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB23132-C137-486F-935F-9D0FA527CA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E0B1D6-CF14-47DF-91F7-DED511F373CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{25DE5334-8C91-426F-A24A-6E4284BCB023}"/>
   </bookViews>
@@ -1894,9 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6EA777-CF04-4C7B-A34F-611A2B3B8ABF}">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="J116" sqref="J116:S118"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>